<commit_message>
Correct mistake in water characterization factors for exiobase water flows.
</commit_message>
<xml_diff>
--- a/Data/Characterization_factors/Regionalized_water_flows_CF_exiobase.xlsx
+++ b/Data/Characterization_factors/Regionalized_water_flows_CF_exiobase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Characterization_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912415D4-2495-4BDC-A252-071D29BCB103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D85D6C-A444-40F5-B3DE-BDDF616E7A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,16 +760,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.2787755370720399</v>
+        <v>1278775.5370720399</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E4">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -777,16 +777,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.2083444675531498</v>
+        <v>2208344.4675531499</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E5">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -794,16 +794,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>27.992197686372801</v>
+        <v>27992197.686372802</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E6">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -811,16 +811,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>76.643163051706907</v>
+        <v>76643163.05170691</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E7">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -828,16 +828,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.89791588968094</v>
+        <v>1897915.88968094</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E8">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -845,16 +845,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.7784352021845899</v>
+        <v>1778435.20218459</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E9">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -862,16 +862,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2.03725481598519</v>
+        <v>2037254.81598519</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E10">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,16 +879,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.32798431569249</v>
+        <v>1327984.31569249</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E11">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -896,16 +896,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>80.760223297116497</v>
+        <v>80760223.297116503</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E12">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -913,16 +913,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.51867463712215</v>
+        <v>1518674.63712215</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E13">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -930,16 +930,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>9.4868125742894893</v>
+        <v>9486812.5742894895</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E14">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -947,16 +947,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>69.360307673216397</v>
+        <v>69360307.673216403</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E15">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -964,16 +964,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1.91704255019405</v>
+        <v>1917042.55019405</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E16">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -981,16 +981,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1.287631032</v>
+        <v>1287631.0319999999</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E17">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -998,16 +998,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1.6357644652808501</v>
+        <v>1635764.46528085</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E18">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1015,16 +1015,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>46.401256857553001</v>
+        <v>46401256.857552998</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E19">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,16 +1032,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.6974411945669099</v>
+        <v>1697441.1945669099</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E20">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,16 +1049,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.990269616673914</v>
+        <v>990269.61667391402</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E21">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1066,16 +1066,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.4579669264199699</v>
+        <v>1457966.9264199699</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E22">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1083,16 +1083,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>68.779982977936896</v>
+        <v>68779982.977936894</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E23">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,16 +1100,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1.5893991641557801</v>
+        <v>1589399.1641557801</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E24">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,16 +1117,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2.1000074092367198</v>
+        <v>2100007.4092367198</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E25">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1134,16 +1134,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>52.2687259047919</v>
+        <v>52268725.904791899</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E26">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1151,16 +1151,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>4.1933750167433104</v>
+        <v>4193375.0167433103</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E27">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1168,16 +1168,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2.77554464870081</v>
+        <v>2775544.64870081</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E28">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1185,16 +1185,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1.1801894477344701</v>
+        <v>1180189.44773447</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E29">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1202,16 +1202,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1.28810053814357</v>
+        <v>1288100.5381435698</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E30">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1219,16 +1219,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3.34107644758679</v>
+        <v>3341076.4475867902</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E31">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1236,16 +1236,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>35.715465431947301</v>
+        <v>35715465.431947298</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E32">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1253,16 +1253,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.59736772318933196</v>
+        <v>597367.72318933194</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E33">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1270,16 +1270,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>45.847278402688197</v>
+        <v>45847278.402688198</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E34">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1287,16 +1287,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>8.3769025234654499</v>
+        <v>8376902.5234654499</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E35">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1304,16 +1304,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.74695800576080895</v>
+        <v>746958.00576080894</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E36">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1321,16 +1321,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>2.6528930606713401</v>
+        <v>2652893.0606713402</v>
       </c>
       <c r="C37" s="2">
-        <v>3.0328358007738071E-7</v>
+        <v>0.30328358007738071</v>
       </c>
       <c r="D37">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E37">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1338,16 +1338,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>30.494259695378599</v>
+        <v>30494259.695378598</v>
       </c>
       <c r="C38" s="2">
-        <v>1.7236479954689801E-5</v>
+        <v>17.236479954689802</v>
       </c>
       <c r="D38">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E38">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1355,16 +1355,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>36.291350814094997</v>
+        <v>36291350.814094998</v>
       </c>
       <c r="C39" s="2">
-        <v>6.8011709257594706E-6</v>
+        <v>6.8011709257594708</v>
       </c>
       <c r="D39">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E39">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1372,16 +1372,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>20.7685786818274</v>
+        <v>20768578.6818274</v>
       </c>
       <c r="C40" s="4">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E40">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1389,16 +1389,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>72.790013380257605</v>
+        <v>72790013.380257607</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E41">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1406,16 +1406,16 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1.3201227254438399</v>
+        <v>1320122.7254438398</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E42">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,16 +1423,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>58.042733717711798</v>
+        <v>58042733.717711799</v>
       </c>
       <c r="C43" s="2">
-        <v>1.3774791108063099E-6</v>
+        <v>1.3774791108063098</v>
       </c>
       <c r="D43">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E43">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1440,16 +1440,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2.0467907660204299</v>
+        <v>2046790.7660204298</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E44">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1457,16 +1457,16 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.69069206468587296</v>
+        <v>690692.06468587299</v>
       </c>
       <c r="C45" s="4">
         <v>0</v>
       </c>
       <c r="D45">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E45">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1474,16 +1474,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>23.935170095642199</v>
+        <v>23935170.095642198</v>
       </c>
       <c r="C46" s="2">
-        <v>1.47735697532199E-6</v>
+        <v>1.47735697532199</v>
       </c>
       <c r="D46">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E46">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1491,16 +1491,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>40.759939233995802</v>
+        <v>40759939.233995803</v>
       </c>
       <c r="C47" s="2">
-        <v>1.754468869154834E-6</v>
+        <v>1.754468869154834</v>
       </c>
       <c r="D47">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E47">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1508,16 +1508,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>44.436430000000001</v>
+        <v>44436430</v>
       </c>
       <c r="C48" s="3">
-        <v>7.0783518702761107E-6</v>
+        <v>7.0783518702761103</v>
       </c>
       <c r="D48">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E48">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1525,16 +1525,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>37.84554</v>
+        <v>37845540</v>
       </c>
       <c r="C49" s="3">
-        <v>2.1218030812236639E-6</v>
+        <v>2.1218030812236641</v>
       </c>
       <c r="D49">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E49">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1542,16 +1542,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>48.950449999999996</v>
+        <v>48950450</v>
       </c>
       <c r="C50" s="3">
-        <v>2.7480373242163938E-7</v>
+        <v>0.27480373242163936</v>
       </c>
       <c r="D50">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E50">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1559,16 +1559,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>73.083860000000001</v>
+        <v>73083860</v>
       </c>
       <c r="C51" s="3">
-        <v>2.0163053305932851E-4</v>
+        <v>201.63053305932851</v>
       </c>
       <c r="D51">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E51">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1576,16 +1576,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>60.263599999999997</v>
+        <v>60263600</v>
       </c>
       <c r="C52" s="3">
-        <v>1.6505819212286619E-6</v>
+        <v>1.6505819212286619</v>
       </c>
       <c r="D52">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E52">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1593,16 +1593,16 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>1.14282777575556</v>
+        <v>1142827.77575556</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E53">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1610,16 +1610,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1.2043175045547301</v>
+        <v>1204317.5045547301</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E54">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,16 +1627,16 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>9.4687043224113907</v>
+        <v>9468704.32241139</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E55">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1644,16 +1644,16 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>48.664218055106801</v>
+        <v>48664218.055106804</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E56">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1661,16 +1661,16 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>1.69254816765644</v>
+        <v>1692548.1676564401</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E57">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1678,16 +1678,16 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>1.1166206479602201</v>
+        <v>1116620.64796022</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E58">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1695,16 +1695,16 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>1.98855064063023</v>
+        <v>1988550.6406302301</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E59">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1712,16 +1712,16 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>1.07126602683724</v>
+        <v>1071266.02683724</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E60">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1729,16 +1729,16 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>31.410730987968801</v>
+        <v>31410730.987968802</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E61">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1746,16 +1746,16 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>1.73175656327926</v>
+        <v>1731756.5632792599</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E62">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1763,16 +1763,16 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>3.0510791476734198</v>
+        <v>3051079.1476734197</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E63">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1780,16 +1780,16 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>28.3478836783312</v>
+        <v>28347883.6783312</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E64">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1797,16 +1797,16 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>1.35379204582823</v>
+        <v>1353792.04582823</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E65">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1814,16 +1814,16 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>1.164123164</v>
+        <v>1164123.1640000001</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E66">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1831,16 +1831,16 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.79191145759964099</v>
+        <v>791911.45759964094</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E67">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1848,16 +1848,16 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>16.678335147979801</v>
+        <v>16678335.147979802</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E68">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1865,16 +1865,16 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>1.26920186822713</v>
+        <v>1269201.86822713</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E69">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1882,16 +1882,16 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.722380839013543</v>
+        <v>722380.83901354298</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E70">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1899,16 +1899,16 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>27.972318656269199</v>
+        <v>27972318.6562692</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E71">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1916,16 +1916,16 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>46.190243855169697</v>
+        <v>46190243.855169699</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E72">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,16 +1933,16 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.95718982602288405</v>
+        <v>957189.82602288399</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E73">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1950,16 +1950,16 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>1.99795340246237</v>
+        <v>1997953.40246237</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E74">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1967,16 +1967,16 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>17.0819146930511</v>
+        <v>17081914.6930511</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E75">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -1984,16 +1984,16 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>1.73690680482118</v>
+        <v>1736906.8048211799</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E76">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2001,16 +2001,16 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>1.6935111265970499</v>
+        <v>1693511.1265970499</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E77">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2018,16 +2018,16 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>1.0872005742566599</v>
+        <v>1087200.57425666</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E78">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2035,16 +2035,16 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>1.19212354964228</v>
+        <v>1192123.54964228</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E79">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2052,16 +2052,16 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>1.24834435213269</v>
+        <v>1248344.3521326899</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E80">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2069,16 +2069,16 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>9.0870762868085908</v>
+        <v>9087076.2868085913</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E81">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2086,16 +2086,16 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.57319141800771001</v>
+        <v>573191.41800771002</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E82">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2103,16 +2103,16 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>27.080652570717302</v>
+        <v>27080652.570717301</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E83">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2120,16 +2120,16 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>2.6855742526188102</v>
+        <v>2685574.2526188102</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E84">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2137,16 +2137,16 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>1.0661120342058299</v>
+        <v>1066112.03420583</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E85">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2154,16 +2154,16 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>1.8989932826631899</v>
+        <v>1898993.2826631898</v>
       </c>
       <c r="C86" s="2">
-        <v>3.0328358007738071E-7</v>
+        <v>0.30328358007738071</v>
       </c>
       <c r="D86">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E86">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2171,16 +2171,16 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>21.306085240363</v>
+        <v>21306085.240363002</v>
       </c>
       <c r="C87" s="2">
-        <v>1.7236479954689801E-5</v>
+        <v>17.236479954689802</v>
       </c>
       <c r="D87">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E87">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2188,16 +2188,16 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>14.450455358702699</v>
+        <v>14450455.358702699</v>
       </c>
       <c r="C88" s="2">
-        <v>6.8011709257594706E-6</v>
+        <v>6.8011709257594708</v>
       </c>
       <c r="D88">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E88">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2205,16 +2205,16 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>3.6628078627846601</v>
+        <v>3662807.86278466</v>
       </c>
       <c r="C89" s="4">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E89">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2222,16 +2222,16 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>25.406232462946399</v>
+        <v>25406232.4629464</v>
       </c>
       <c r="C90" s="4">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E90">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2239,16 +2239,16 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.737323233301721</v>
+        <v>737323.23330172105</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E91">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2256,16 +2256,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>22.240873456833601</v>
+        <v>22240873.456833601</v>
       </c>
       <c r="C92" s="2">
-        <v>1.3774791108063099E-6</v>
+        <v>1.3774791108063098</v>
       </c>
       <c r="D92">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E92">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2273,16 +2273,16 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>2.61374499996661</v>
+        <v>2613744.9999666102</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E93">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2290,16 +2290,16 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.77994974039124998</v>
+        <v>779949.74039125</v>
       </c>
       <c r="C94" s="4">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E94">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2307,16 +2307,16 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>8.9257606089114194</v>
+        <v>8925760.6089114193</v>
       </c>
       <c r="C95" s="2">
-        <v>1.47735697532199E-6</v>
+        <v>1.47735697532199</v>
       </c>
       <c r="D95">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E95">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -2324,16 +2324,16 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>21.1343487298507</v>
+        <v>21134348.729850698</v>
       </c>
       <c r="C96" s="2">
-        <v>1.754468869154834E-6</v>
+        <v>1.754468869154834</v>
       </c>
       <c r="D96">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E96">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -2341,16 +2341,16 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>22.84553</v>
+        <v>22845530</v>
       </c>
       <c r="C97" s="3">
-        <v>7.0783518702761107E-6</v>
+        <v>7.0783518702761103</v>
       </c>
       <c r="D97">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E97">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2358,16 +2358,16 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>6.3476400000000002</v>
+        <v>6347640</v>
       </c>
       <c r="C98" s="3">
-        <v>2.1218030812236639E-6</v>
+        <v>2.1218030812236641</v>
       </c>
       <c r="D98">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E98">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2375,16 +2375,16 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5.9185800000000004</v>
+        <v>5918580</v>
       </c>
       <c r="C99" s="3">
-        <v>2.7480373242163938E-7</v>
+        <v>0.27480373242163936</v>
       </c>
       <c r="D99">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E99">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2392,16 +2392,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>59.28154</v>
+        <v>59281540</v>
       </c>
       <c r="C100" s="3">
-        <v>2.0163053305932851E-4</v>
+        <v>201.63053305932851</v>
       </c>
       <c r="D100">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E100">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2409,16 +2409,16 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>40.970869999999998</v>
+        <v>40970870</v>
       </c>
       <c r="C101" s="3">
-        <v>1.6505819212286619E-6</v>
+        <v>1.6505819212286619</v>
       </c>
       <c r="D101">
-        <v>3.0620000000000002E-4</v>
+        <v>306.2</v>
       </c>
       <c r="E101">
-        <v>0.105</v>
+        <v>105000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.10 update: data for 2021 + better documentation
</commit_message>
<xml_diff>
--- a/Data/Characterization_factors/Regionalized_water_flows_CF_exiobase.xlsx
+++ b/Data/Characterization_factors/Regionalized_water_flows_CF_exiobase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Characterization_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D85D6C-A444-40F5-B3DE-BDDF616E7A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FBE876-DF3A-4D77-8977-7DDCB511A377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,12 +717,13 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -760,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1278775.5370720399</v>
+        <v>2140000</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -769,7 +770,7 @@
         <v>306.2</v>
       </c>
       <c r="E4">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -777,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2208344.4675531499</v>
+        <v>4770000</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -786,7 +787,7 @@
         <v>306.2</v>
       </c>
       <c r="E5">
-        <v>105000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -794,16 +795,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>27992197.686372802</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>59400000</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6.7100000000000001E-7</v>
       </c>
       <c r="D6">
         <v>306.2</v>
       </c>
       <c r="E6">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -811,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>76643163.05170691</v>
+        <v>95700000</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -820,7 +821,7 @@
         <v>306.2</v>
       </c>
       <c r="E7">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -828,7 +829,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1897915.88968094</v>
+        <v>3340000</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -837,7 +838,7 @@
         <v>306.2</v>
       </c>
       <c r="E8">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -845,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1778435.20218459</v>
+        <v>2920000</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -854,7 +855,7 @@
         <v>306.2</v>
       </c>
       <c r="E9">
-        <v>105000</v>
+        <v>159600</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -862,7 +863,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2037254.81598519</v>
+        <v>2700000</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -871,7 +872,7 @@
         <v>306.2</v>
       </c>
       <c r="E10">
-        <v>105000</v>
+        <v>140700</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,7 +880,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1327984.31569249</v>
+        <v>2030000</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -888,7 +889,7 @@
         <v>306.2</v>
       </c>
       <c r="E11">
-        <v>105000</v>
+        <v>94500</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -896,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>80760223.297116503</v>
+        <v>74900000</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -905,7 +906,7 @@
         <v>306.2</v>
       </c>
       <c r="E12">
-        <v>105000</v>
+        <v>46200</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -913,7 +914,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1518674.63712215</v>
+        <v>2280000</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -922,7 +923,7 @@
         <v>306.2</v>
       </c>
       <c r="E13">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -930,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>9486812.5742894895</v>
+        <v>15800000</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -947,7 +948,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>69360307.673216403</v>
+        <v>85100000</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -956,7 +957,7 @@
         <v>306.2</v>
       </c>
       <c r="E15">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -964,7 +965,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1917042.55019405</v>
+        <v>2680000</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -973,7 +974,7 @@
         <v>306.2</v>
       </c>
       <c r="E16">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -981,7 +982,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1287631.0319999999</v>
+        <v>2380000</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -990,7 +991,7 @@
         <v>306.2</v>
       </c>
       <c r="E17">
-        <v>105000</v>
+        <v>69300</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -998,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1635764.46528085</v>
+        <v>2560000</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1007,7 +1008,7 @@
         <v>306.2</v>
       </c>
       <c r="E18">
-        <v>105000</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1015,7 +1016,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>46401256.857552998</v>
+        <v>51900000</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1024,7 +1025,7 @@
         <v>306.2</v>
       </c>
       <c r="E19">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,7 +1033,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1697441.1945669099</v>
+        <v>2810000</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1041,7 +1042,7 @@
         <v>306.2</v>
       </c>
       <c r="E20">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>990269.61667391402</v>
+        <v>1660000</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1058,7 +1059,7 @@
         <v>306.2</v>
       </c>
       <c r="E21">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1066,7 +1067,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1457966.9264199699</v>
+        <v>2230000</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1075,7 +1076,7 @@
         <v>306.2</v>
       </c>
       <c r="E22">
-        <v>105000</v>
+        <v>84000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1083,7 +1084,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>68779982.977936894</v>
+        <v>10700000</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1092,7 +1093,7 @@
         <v>306.2</v>
       </c>
       <c r="E23">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,7 +1101,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1589399.1641557801</v>
+        <v>2170000</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1109,7 +1110,7 @@
         <v>306.2</v>
       </c>
       <c r="E24">
-        <v>105000</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,7 +1118,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2100007.4092367198</v>
+        <v>3000000</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1126,7 +1127,7 @@
         <v>306.2</v>
       </c>
       <c r="E25">
-        <v>105000</v>
+        <v>79800</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1134,7 +1135,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>52268725.904791899</v>
+        <v>45800000</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1143,7 +1144,7 @@
         <v>306.2</v>
       </c>
       <c r="E26">
-        <v>105000</v>
+        <v>29400</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1151,7 +1152,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>4193375.0167433103</v>
+        <v>6710000</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1160,7 +1161,7 @@
         <v>306.2</v>
       </c>
       <c r="E27">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1168,7 +1169,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2775544.64870081</v>
+        <v>3700000</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1177,7 +1178,7 @@
         <v>306.2</v>
       </c>
       <c r="E28">
-        <v>105000</v>
+        <v>69300</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1185,7 +1186,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1180189.44773447</v>
+        <v>2020000</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1194,7 +1195,7 @@
         <v>306.2</v>
       </c>
       <c r="E29">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1202,7 +1203,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1288100.5381435698</v>
+        <v>2130000</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1211,7 +1212,7 @@
         <v>306.2</v>
       </c>
       <c r="E30">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1219,7 +1220,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3341076.4475867902</v>
+        <v>14900000</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1228,7 +1229,7 @@
         <v>306.2</v>
       </c>
       <c r="E31">
-        <v>105000</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1236,7 +1237,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>35715465.431947298</v>
+        <v>37400000</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1245,7 +1246,7 @@
         <v>306.2</v>
       </c>
       <c r="E32">
-        <v>105000</v>
+        <v>67200</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1253,7 +1254,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>597367.72318933194</v>
+        <v>864000</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1262,7 +1263,7 @@
         <v>306.2</v>
       </c>
       <c r="E33">
-        <v>105000</v>
+        <v>136500</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1270,16 +1271,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>45847278.402688198</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
+        <v>25700000</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3.58E-6</v>
       </c>
       <c r="D34">
         <v>306.2</v>
       </c>
       <c r="E34">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1287,7 +1288,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>8376902.5234654499</v>
+        <v>9650000</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1296,7 +1297,7 @@
         <v>306.2</v>
       </c>
       <c r="E35">
-        <v>105000</v>
+        <v>79800</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1304,7 +1305,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>746958.00576080894</v>
+        <v>973000</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1313,7 +1314,7 @@
         <v>306.2</v>
       </c>
       <c r="E36">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1321,16 +1322,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>2652893.0606713402</v>
+        <v>6350000</v>
       </c>
       <c r="C37" s="2">
-        <v>0.30328358007738071</v>
+        <v>8.2600000000000001E-7</v>
       </c>
       <c r="D37">
         <v>306.2</v>
       </c>
       <c r="E37">
-        <v>105000</v>
+        <v>100800</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1338,16 +1339,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>30494259.695378598</v>
+        <v>35900000</v>
       </c>
       <c r="C38" s="2">
-        <v>17.236479954689802</v>
+        <v>5.0399999999999999E-5</v>
       </c>
       <c r="D38">
         <v>306.2</v>
       </c>
       <c r="E38">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1355,16 +1356,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>36291350.814094998</v>
+        <v>41800000</v>
       </c>
       <c r="C39" s="2">
-        <v>6.8011709257594708</v>
+        <v>1.7499999999999998E-5</v>
       </c>
       <c r="D39">
         <v>306.2</v>
       </c>
       <c r="E39">
-        <v>105000</v>
+        <v>50400</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1372,16 +1373,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>20768578.6818274</v>
-      </c>
-      <c r="C40" s="4">
-        <v>0</v>
+        <v>16500000</v>
+      </c>
+      <c r="C40" s="2">
+        <v>3.5499999999999999E-7</v>
       </c>
       <c r="D40">
         <v>306.2</v>
       </c>
       <c r="E40">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1389,7 +1390,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>72790013.380257607</v>
+        <v>81600000</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -1398,7 +1399,7 @@
         <v>306.2</v>
       </c>
       <c r="E41">
-        <v>105000</v>
+        <v>86100</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1406,7 +1407,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1320122.7254438398</v>
+        <v>2070000</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1415,7 +1416,7 @@
         <v>306.2</v>
       </c>
       <c r="E42">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,16 +1424,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>58042733.717711799</v>
+        <v>70700000</v>
       </c>
       <c r="C43" s="2">
-        <v>1.3774791108063098</v>
+        <v>1.17E-5</v>
       </c>
       <c r="D43">
         <v>306.2</v>
       </c>
       <c r="E43">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1440,16 +1441,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2046790.7660204298</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
+        <v>10400000</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1.0300000000000001E-6</v>
       </c>
       <c r="D44">
         <v>306.2</v>
       </c>
       <c r="E44">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1457,7 +1458,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>690692.06468587299</v>
+        <v>713000</v>
       </c>
       <c r="C45" s="4">
         <v>0</v>
@@ -1466,7 +1467,7 @@
         <v>306.2</v>
       </c>
       <c r="E45">
-        <v>105000</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1474,16 +1475,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>23935170.095642198</v>
+        <v>25100000</v>
       </c>
       <c r="C46" s="2">
-        <v>1.47735697532199</v>
+        <v>3.7500000000000001E-6</v>
       </c>
       <c r="D46">
         <v>306.2</v>
       </c>
       <c r="E46">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1491,16 +1492,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>40759939.233995803</v>
+        <v>68500000</v>
       </c>
       <c r="C47" s="2">
-        <v>1.754468869154834</v>
+        <v>1.0200000000000001E-5</v>
       </c>
       <c r="D47">
         <v>306.2</v>
       </c>
       <c r="E47">
-        <v>105000</v>
+        <v>73500</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1508,16 +1509,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>44436430</v>
+        <v>39100000</v>
       </c>
       <c r="C48" s="3">
-        <v>7.0783518702761103</v>
+        <v>2.7399999999999999E-5</v>
       </c>
       <c r="D48">
         <v>306.2</v>
       </c>
       <c r="E48">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1525,16 +1526,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>37845540</v>
+        <v>34600000</v>
       </c>
       <c r="C49" s="3">
-        <v>2.1218030812236641</v>
+        <v>8.0900000000000005E-6</v>
       </c>
       <c r="D49">
         <v>306.2</v>
       </c>
       <c r="E49">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1542,16 +1543,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>48950450</v>
+        <v>56100000</v>
       </c>
       <c r="C50" s="3">
-        <v>0.27480373242163936</v>
+        <v>6.7999999999999995E-7</v>
       </c>
       <c r="D50">
         <v>306.2</v>
       </c>
       <c r="E50">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1559,16 +1560,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>73083860</v>
+        <v>76200000</v>
       </c>
       <c r="C51" s="3">
-        <v>201.63053305932851</v>
+        <v>2.42E-4</v>
       </c>
       <c r="D51">
         <v>306.2</v>
       </c>
       <c r="E51">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1576,16 +1577,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>60263600</v>
+        <v>68800000</v>
       </c>
       <c r="C52" s="3">
-        <v>1.6505819212286619</v>
+        <v>3.0800000000000003E-5</v>
       </c>
       <c r="D52">
         <v>306.2</v>
       </c>
       <c r="E52">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1593,7 +1594,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>1142827.77575556</v>
+        <v>2060000</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1602,7 +1603,7 @@
         <v>306.2</v>
       </c>
       <c r="E53">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1610,7 +1611,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1204317.5045547301</v>
+        <v>3520000</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1619,7 +1620,7 @@
         <v>306.2</v>
       </c>
       <c r="E54">
-        <v>105000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,16 +1628,16 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>9468704.32241139</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
+        <v>10600000</v>
+      </c>
+      <c r="C55" s="3">
+        <v>6.7100000000000001E-7</v>
       </c>
       <c r="D55">
         <v>306.2</v>
       </c>
       <c r="E55">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1644,7 +1645,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>48664218.055106804</v>
+        <v>62400000</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1653,7 +1654,7 @@
         <v>306.2</v>
       </c>
       <c r="E56">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1661,7 +1662,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>1692548.1676564401</v>
+        <v>3140000</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1670,7 +1671,7 @@
         <v>306.2</v>
       </c>
       <c r="E57">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1678,7 +1679,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>1116620.64796022</v>
+        <v>2090000</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1687,7 +1688,7 @@
         <v>306.2</v>
       </c>
       <c r="E58">
-        <v>105000</v>
+        <v>159600</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1695,7 +1696,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>1988550.6406302301</v>
+        <v>2120000</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1704,7 +1705,7 @@
         <v>306.2</v>
       </c>
       <c r="E59">
-        <v>105000</v>
+        <v>140700</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1712,7 +1713,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>1071266.02683724</v>
+        <v>1870000</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1721,7 +1722,7 @@
         <v>306.2</v>
       </c>
       <c r="E60">
-        <v>105000</v>
+        <v>94500</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1729,7 +1730,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>31410730.987968802</v>
+        <v>35500000</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1738,7 +1739,7 @@
         <v>306.2</v>
       </c>
       <c r="E61">
-        <v>105000</v>
+        <v>46200</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1746,7 +1747,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>1731756.5632792599</v>
+        <v>2160000</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1755,7 +1756,7 @@
         <v>306.2</v>
       </c>
       <c r="E62">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1763,7 +1764,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>3051079.1476734197</v>
+        <v>4990000</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1780,7 +1781,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>28347883.6783312</v>
+        <v>40200000</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1789,7 +1790,7 @@
         <v>306.2</v>
       </c>
       <c r="E64">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1797,7 +1798,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>1353792.04582823</v>
+        <v>1980000</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1806,7 +1807,7 @@
         <v>306.2</v>
       </c>
       <c r="E65">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1814,7 +1815,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>1164123.1640000001</v>
+        <v>2090000</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1823,7 +1824,7 @@
         <v>306.2</v>
       </c>
       <c r="E66">
-        <v>105000</v>
+        <v>69300</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1831,7 +1832,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>791911.45759964094</v>
+        <v>1170000</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,7 +1841,7 @@
         <v>306.2</v>
       </c>
       <c r="E67">
-        <v>105000</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1848,7 +1849,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>16678335.147979802</v>
+        <v>19000000</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1857,7 +1858,7 @@
         <v>306.2</v>
       </c>
       <c r="E68">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1865,7 +1866,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>1269201.86822713</v>
+        <v>2270000</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1874,7 +1875,7 @@
         <v>306.2</v>
       </c>
       <c r="E69">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1882,7 +1883,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>722380.83901354298</v>
+        <v>1400000</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1891,7 +1892,7 @@
         <v>306.2</v>
       </c>
       <c r="E70">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1899,7 +1900,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>27972318.6562692</v>
+        <v>1900000</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1908,7 +1909,7 @@
         <v>306.2</v>
       </c>
       <c r="E71">
-        <v>105000</v>
+        <v>84000</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1916,7 +1917,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>46190243.855169699</v>
+        <v>4950000</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1925,7 +1926,7 @@
         <v>306.2</v>
       </c>
       <c r="E72">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,7 +1934,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>957189.82602288399</v>
+        <v>1860000</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1942,7 +1943,7 @@
         <v>306.2</v>
       </c>
       <c r="E73">
-        <v>105000</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1950,7 +1951,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>1997953.40246237</v>
+        <v>3160000</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1959,7 +1960,7 @@
         <v>306.2</v>
       </c>
       <c r="E74">
-        <v>105000</v>
+        <v>79800</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1967,7 +1968,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>17081914.6930511</v>
+        <v>19200000</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1976,7 +1977,7 @@
         <v>306.2</v>
       </c>
       <c r="E75">
-        <v>105000</v>
+        <v>29400</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -1984,7 +1985,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>1736906.8048211799</v>
+        <v>3020000</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -1993,7 +1994,7 @@
         <v>306.2</v>
       </c>
       <c r="E76">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2001,7 +2002,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>1693511.1265970499</v>
+        <v>2170000</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2010,7 +2011,7 @@
         <v>306.2</v>
       </c>
       <c r="E77">
-        <v>105000</v>
+        <v>69300</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2018,7 +2019,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>1087200.57425666</v>
+        <v>1950000</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2027,7 +2028,7 @@
         <v>306.2</v>
       </c>
       <c r="E78">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2035,7 +2036,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>1192123.54964228</v>
+        <v>2130000</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2044,7 +2045,7 @@
         <v>306.2</v>
       </c>
       <c r="E79">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2052,7 +2053,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>1248344.3521326899</v>
+        <v>2290000</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2061,7 +2062,7 @@
         <v>306.2</v>
       </c>
       <c r="E80">
-        <v>105000</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2069,7 +2070,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>9087076.2868085913</v>
+        <v>11300000</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2078,7 +2079,7 @@
         <v>306.2</v>
       </c>
       <c r="E81">
-        <v>105000</v>
+        <v>67200</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2086,7 +2087,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>573191.41800771002</v>
+        <v>637000</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2095,7 +2096,7 @@
         <v>306.2</v>
       </c>
       <c r="E82">
-        <v>105000</v>
+        <v>136500</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2103,16 +2104,16 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>27080652.570717301</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
+        <v>6290000</v>
+      </c>
+      <c r="C83" s="3">
+        <v>3.58E-6</v>
       </c>
       <c r="D83">
         <v>306.2</v>
       </c>
       <c r="E83">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2120,7 +2121,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>2685574.2526188102</v>
+        <v>2970000</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2129,7 +2130,7 @@
         <v>306.2</v>
       </c>
       <c r="E84">
-        <v>105000</v>
+        <v>79800</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2137,7 +2138,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>1066112.03420583</v>
+        <v>1650000</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2146,7 +2147,7 @@
         <v>306.2</v>
       </c>
       <c r="E85">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2154,16 +2155,16 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>1898993.2826631898</v>
+        <v>4380000</v>
       </c>
       <c r="C86" s="2">
-        <v>0.30328358007738071</v>
+        <v>8.2600000000000001E-7</v>
       </c>
       <c r="D86">
         <v>306.2</v>
       </c>
       <c r="E86">
-        <v>105000</v>
+        <v>100800</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2171,16 +2172,16 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>21306085.240363002</v>
+        <v>37900000</v>
       </c>
       <c r="C87" s="2">
-        <v>17.236479954689802</v>
+        <v>5.0399999999999999E-5</v>
       </c>
       <c r="D87">
         <v>306.2</v>
       </c>
       <c r="E87">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2188,16 +2189,16 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>14450455.358702699</v>
+        <v>20300000</v>
       </c>
       <c r="C88" s="2">
-        <v>6.8011709257594708</v>
+        <v>1.7499999999999998E-5</v>
       </c>
       <c r="D88">
         <v>306.2</v>
       </c>
       <c r="E88">
-        <v>105000</v>
+        <v>50400</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2205,16 +2206,16 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>3662807.86278466</v>
-      </c>
-      <c r="C89" s="4">
-        <v>0</v>
+        <v>4480000</v>
+      </c>
+      <c r="C89" s="2">
+        <v>3.5499999999999999E-7</v>
       </c>
       <c r="D89">
         <v>306.2</v>
       </c>
       <c r="E89">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2222,7 +2223,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>25406232.4629464</v>
+        <v>34100000</v>
       </c>
       <c r="C90" s="4">
         <v>0</v>
@@ -2231,7 +2232,7 @@
         <v>306.2</v>
       </c>
       <c r="E90">
-        <v>105000</v>
+        <v>86100</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2239,7 +2240,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>737323.23330172105</v>
+        <v>1380000</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2248,7 +2249,7 @@
         <v>306.2</v>
       </c>
       <c r="E91">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2256,16 +2257,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>22240873.456833601</v>
+        <v>25100000</v>
       </c>
       <c r="C92" s="2">
-        <v>1.3774791108063098</v>
+        <v>1.17E-5</v>
       </c>
       <c r="D92">
         <v>306.2</v>
       </c>
       <c r="E92">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2273,16 +2274,16 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>2613744.9999666102</v>
-      </c>
-      <c r="C93">
-        <v>0</v>
+        <v>6880000</v>
+      </c>
+      <c r="C93" s="3">
+        <v>1.0300000000000001E-6</v>
       </c>
       <c r="D93">
         <v>306.2</v>
       </c>
       <c r="E93">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2290,7 +2291,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>779949.74039125</v>
+        <v>744000</v>
       </c>
       <c r="C94" s="4">
         <v>0</v>
@@ -2299,7 +2300,7 @@
         <v>306.2</v>
       </c>
       <c r="E94">
-        <v>105000</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2307,16 +2308,16 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>8925760.6089114193</v>
+        <v>9070000</v>
       </c>
       <c r="C95" s="2">
-        <v>1.47735697532199</v>
+        <v>3.7500000000000001E-6</v>
       </c>
       <c r="D95">
         <v>306.2</v>
       </c>
       <c r="E95">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -2324,16 +2325,16 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>21134348.729850698</v>
+        <v>49800000</v>
       </c>
       <c r="C96" s="2">
-        <v>1.754468869154834</v>
+        <v>1.0200000000000001E-5</v>
       </c>
       <c r="D96">
         <v>306.2</v>
       </c>
       <c r="E96">
-        <v>105000</v>
+        <v>73500</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -2341,16 +2342,16 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>22845530</v>
+        <v>18700000</v>
       </c>
       <c r="C97" s="3">
-        <v>7.0783518702761103</v>
+        <v>2.7399999999999999E-5</v>
       </c>
       <c r="D97">
         <v>306.2</v>
       </c>
       <c r="E97">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2358,16 +2359,16 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>6347640</v>
+        <v>9600000</v>
       </c>
       <c r="C98" s="3">
-        <v>2.1218030812236641</v>
+        <v>8.0900000000000005E-6</v>
       </c>
       <c r="D98">
         <v>306.2</v>
       </c>
       <c r="E98">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2375,16 +2376,16 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5918580</v>
+        <v>6640000</v>
       </c>
       <c r="C99" s="3">
-        <v>0.27480373242163936</v>
+        <v>6.7999999999999995E-7</v>
       </c>
       <c r="D99">
         <v>306.2</v>
       </c>
       <c r="E99">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2392,16 +2393,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>59281540</v>
+        <v>52000000</v>
       </c>
       <c r="C100" s="3">
-        <v>201.63053305932851</v>
+        <v>2.42E-4</v>
       </c>
       <c r="D100">
         <v>306.2</v>
       </c>
       <c r="E100">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2409,16 +2410,16 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>40970870</v>
+        <v>45000000</v>
       </c>
       <c r="C101" s="3">
-        <v>1.6505819212286619</v>
+        <v>3.0800000000000003E-5</v>
       </c>
       <c r="D101">
         <v>306.2</v>
       </c>
       <c r="E101">
-        <v>105000</v>
+        <v>42000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally made it work for 2022 as well!
</commit_message>
<xml_diff>
--- a/Data/Characterization_factors/Regionalized_water_flows_CF_exiobase.xlsx
+++ b/Data/Characterization_factors/Regionalized_water_flows_CF_exiobase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Characterization_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FBE876-DF3A-4D77-8977-7DDCB511A377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDF51D8-DC5C-4801-93D9-A3086A9C9877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,7 +717,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>